<commit_message>
finished and updated assn 3
</commit_message>
<xml_diff>
--- a/assignments/Excel Lab - Week 4 - Homework Assignment_Part1.xlsx
+++ b/assignments/Excel Lab - Week 4 - Homework Assignment_Part1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens_Institute_NJ\TA-Sem1-Form\Lab Recitation E\Week 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Humna\Documents\GitHub\mis201\assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA914649-B53E-45A5-942A-D4B125FC7ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BA5126-F255-459F-9570-AAC2513718A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="11" xr2:uid="{ADEAAF85-69B3-4B7C-BFE7-E14DCD3C3FB1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ADEAAF85-69B3-4B7C-BFE7-E14DCD3C3FB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Q1. Summary of Sales" sheetId="1" r:id="rId1"/>
@@ -38,8 +38,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -47,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="59">
   <si>
     <t xml:space="preserve">Destination </t>
   </si>
@@ -266,15 +264,19 @@
   <si>
     <t xml:space="preserve"> For 2.  Create A Validation that will only accept values from C++, Python, R, Java (+Any other language you want to add)</t>
   </si>
+  <si>
+    <t>Totals:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -522,31 +524,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -565,10 +552,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -586,25 +573,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -615,6 +584,63 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -932,310 +958,597 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E6CBEC-4107-4F85-BB35-04C81007C7A1}">
   <dimension ref="A2:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" customWidth="1"/>
-    <col min="12" max="12" width="11.77734375" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" width="11.90625" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="5" width="14.90625" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" customWidth="1"/>
+    <col min="13" max="13" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:14" ht="34.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="2" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="B7" s="29">
+        <v>82875</v>
+      </c>
+      <c r="C7" s="32">
+        <v>15937.5</v>
+      </c>
+      <c r="D7" s="32">
+        <v>10800</v>
+      </c>
+      <c r="E7" s="32">
+        <v>16625</v>
+      </c>
+      <c r="F7" s="32">
+        <v>6937.5</v>
+      </c>
+      <c r="G7" s="32">
+        <v>3847.5</v>
+      </c>
+      <c r="H7" s="35">
+        <v>33400</v>
+      </c>
+      <c r="I7" s="35">
+        <v>45025</v>
+      </c>
+      <c r="J7" s="35">
+        <v>17030</v>
+      </c>
+      <c r="K7" s="35">
+        <v>19600</v>
+      </c>
+      <c r="L7" s="35">
+        <v>28600</v>
+      </c>
+      <c r="M7" s="35">
+        <v>27000</v>
+      </c>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="B8" s="30">
+        <v>42500</v>
+      </c>
+      <c r="C8" s="33">
+        <v>19910</v>
+      </c>
+      <c r="D8" s="33">
+        <v>53125</v>
+      </c>
+      <c r="E8" s="33">
+        <v>14910</v>
+      </c>
+      <c r="F8" s="33">
+        <v>6277.5</v>
+      </c>
+      <c r="G8" s="33">
+        <v>4425</v>
+      </c>
+      <c r="H8" s="36">
+        <v>36500</v>
+      </c>
+      <c r="I8" s="36">
+        <v>33000</v>
+      </c>
+      <c r="J8" s="36">
+        <v>20700</v>
+      </c>
+      <c r="K8" s="36">
+        <v>24650</v>
+      </c>
+      <c r="L8" s="36">
+        <v>32200</v>
+      </c>
+      <c r="M8" s="36">
+        <v>31300</v>
+      </c>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="B9" s="30">
+        <v>24150</v>
+      </c>
+      <c r="C9" s="33">
+        <v>7425</v>
+      </c>
+      <c r="D9" s="33">
+        <v>23750</v>
+      </c>
+      <c r="E9" s="33">
+        <v>18150</v>
+      </c>
+      <c r="F9" s="33">
+        <v>14910</v>
+      </c>
+      <c r="G9" s="33">
+        <v>17250</v>
+      </c>
+      <c r="H9" s="36">
+        <v>31300</v>
+      </c>
+      <c r="I9" s="36">
+        <v>34000</v>
+      </c>
+      <c r="J9" s="36">
+        <v>18030</v>
+      </c>
+      <c r="K9" s="36">
+        <v>29500</v>
+      </c>
+      <c r="L9" s="36">
+        <v>45025</v>
+      </c>
+      <c r="M9" s="36">
+        <v>35000</v>
+      </c>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="B10" s="30">
+        <v>22575</v>
+      </c>
+      <c r="C10" s="33">
+        <v>10353</v>
+      </c>
+      <c r="D10" s="33">
+        <v>7062.5</v>
+      </c>
+      <c r="E10" s="33">
+        <v>7425</v>
+      </c>
+      <c r="F10" s="33">
+        <v>58800</v>
+      </c>
+      <c r="G10" s="33">
+        <v>5292.5</v>
+      </c>
+      <c r="H10" s="36">
+        <v>35600</v>
+      </c>
+      <c r="I10" s="36">
+        <v>39299</v>
+      </c>
+      <c r="J10" s="36">
+        <v>19600</v>
+      </c>
+      <c r="K10" s="36">
+        <v>25500</v>
+      </c>
+      <c r="L10" s="36">
+        <v>45025</v>
+      </c>
+      <c r="M10" s="36">
+        <v>45000</v>
+      </c>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="B11" s="30">
+        <v>23625</v>
+      </c>
+      <c r="C11" s="33">
+        <v>6875</v>
+      </c>
+      <c r="D11" s="33">
+        <v>17040</v>
+      </c>
+      <c r="E11" s="33">
+        <v>6562.5</v>
+      </c>
+      <c r="F11" s="33">
+        <v>61625</v>
+      </c>
+      <c r="G11" s="33">
+        <v>7245.25</v>
+      </c>
+      <c r="H11" s="36">
+        <v>37557</v>
+      </c>
+      <c r="I11" s="36">
+        <v>35851</v>
+      </c>
+      <c r="J11" s="36">
+        <v>24455</v>
+      </c>
+      <c r="K11" s="36">
+        <v>25000</v>
+      </c>
+      <c r="L11" s="36">
+        <v>28000</v>
+      </c>
+      <c r="M11" s="36">
+        <v>45025</v>
+      </c>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="B12" s="30">
+        <v>19250</v>
+      </c>
+      <c r="C12" s="33">
+        <v>15750</v>
+      </c>
+      <c r="D12" s="33">
+        <v>7837.5</v>
+      </c>
+      <c r="E12" s="33">
+        <v>6075</v>
+      </c>
+      <c r="F12" s="33">
+        <v>6750</v>
+      </c>
+      <c r="G12" s="33">
+        <v>13650</v>
+      </c>
+      <c r="H12" s="36">
+        <v>31300</v>
+      </c>
+      <c r="I12" s="36">
+        <v>35600</v>
+      </c>
+      <c r="J12" s="36">
+        <v>25500</v>
+      </c>
+      <c r="K12" s="36">
+        <v>27316</v>
+      </c>
+      <c r="L12" s="36">
+        <v>28000</v>
+      </c>
+      <c r="M12" s="36">
+        <v>45025</v>
+      </c>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="B13" s="30">
+        <v>9000</v>
+      </c>
+      <c r="C13" s="33">
+        <v>8002.5</v>
+      </c>
+      <c r="D13" s="33">
+        <v>63750</v>
+      </c>
+      <c r="E13" s="33">
+        <v>15087.5</v>
+      </c>
+      <c r="F13" s="33">
+        <v>42000</v>
+      </c>
+      <c r="G13" s="33">
+        <v>3562.5</v>
+      </c>
+      <c r="H13" s="36">
+        <v>28000</v>
+      </c>
+      <c r="I13" s="36">
+        <v>43579</v>
+      </c>
+      <c r="J13" s="36">
+        <v>29155</v>
+      </c>
+      <c r="K13" s="36">
+        <v>33000</v>
+      </c>
+      <c r="L13" s="36">
+        <v>22300</v>
+      </c>
+      <c r="M13" s="36">
+        <v>45000</v>
+      </c>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="B14" s="30">
+        <v>3185.0000000000005</v>
+      </c>
+      <c r="C14" s="33">
+        <v>15562.5</v>
+      </c>
+      <c r="D14" s="33">
+        <v>6781.25</v>
+      </c>
+      <c r="E14" s="33">
+        <v>63000</v>
+      </c>
+      <c r="F14" s="33">
+        <v>4562.5</v>
+      </c>
+      <c r="G14" s="33">
+        <v>3300</v>
+      </c>
+      <c r="H14" s="36">
+        <v>45025</v>
+      </c>
+      <c r="I14" s="36">
+        <v>33856</v>
+      </c>
+      <c r="J14" s="36">
+        <v>30400</v>
+      </c>
+      <c r="K14" s="36">
+        <v>25200</v>
+      </c>
+      <c r="L14" s="36">
+        <v>33400</v>
+      </c>
+      <c r="M14" s="36">
+        <v>45025</v>
+      </c>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+      <c r="B15" s="30">
+        <v>23625</v>
+      </c>
+      <c r="C15" s="33">
+        <v>65875</v>
+      </c>
+      <c r="D15" s="33">
+        <v>16276.75</v>
+      </c>
+      <c r="E15" s="33">
+        <v>6125</v>
+      </c>
+      <c r="F15" s="33">
+        <v>7062.5</v>
+      </c>
+      <c r="G15" s="33">
+        <v>16330</v>
+      </c>
+      <c r="H15" s="36">
+        <v>28618</v>
+      </c>
+      <c r="I15" s="36">
+        <v>31300</v>
+      </c>
+      <c r="J15" s="36">
+        <v>24650</v>
+      </c>
+      <c r="K15" s="36">
+        <v>45025</v>
+      </c>
+      <c r="L15" s="36">
+        <v>29000</v>
+      </c>
+      <c r="M15" s="36">
+        <v>40940</v>
+      </c>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="4"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="B16" s="31">
+        <v>7000</v>
+      </c>
+      <c r="C16" s="34">
+        <v>38250</v>
+      </c>
+      <c r="D16" s="34">
+        <v>2940</v>
+      </c>
+      <c r="E16" s="34">
+        <v>3705</v>
+      </c>
+      <c r="F16" s="34">
+        <v>76500</v>
+      </c>
+      <c r="G16" s="34">
+        <v>5365.5</v>
+      </c>
+      <c r="H16" s="37">
+        <v>35600</v>
+      </c>
+      <c r="I16" s="37">
+        <v>34000</v>
+      </c>
+      <c r="J16" s="37">
+        <v>27500</v>
+      </c>
+      <c r="K16" s="37">
+        <v>28000</v>
+      </c>
+      <c r="L16" s="37">
+        <v>35851</v>
+      </c>
+      <c r="M16" s="37">
+        <v>31160</v>
+      </c>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="B17" s="38">
+        <f>SUM(B7:B16)</f>
+        <v>257785</v>
+      </c>
+      <c r="C17" s="38">
+        <f>SUM(C7:C16)</f>
+        <v>203940.5</v>
+      </c>
+      <c r="D17" s="38">
+        <f t="shared" ref="D17:M17" si="0">SUM(D7:D16)</f>
+        <v>209363</v>
+      </c>
+      <c r="E17" s="38">
+        <f t="shared" si="0"/>
+        <v>157665</v>
+      </c>
+      <c r="F17" s="38">
+        <f t="shared" si="0"/>
+        <v>285425</v>
+      </c>
+      <c r="G17" s="38">
+        <f t="shared" si="0"/>
+        <v>80268.25</v>
+      </c>
+      <c r="H17" s="38">
+        <f t="shared" si="0"/>
+        <v>342900</v>
+      </c>
+      <c r="I17" s="38">
+        <f t="shared" si="0"/>
+        <v>365510</v>
+      </c>
+      <c r="J17" s="38">
+        <f t="shared" si="0"/>
+        <v>237020</v>
+      </c>
+      <c r="K17" s="38">
+        <f t="shared" si="0"/>
+        <v>282791</v>
+      </c>
+      <c r="L17" s="38">
+        <f t="shared" si="0"/>
+        <v>327401</v>
+      </c>
+      <c r="M17" s="38">
+        <f t="shared" si="0"/>
+        <v>390475</v>
+      </c>
+      <c r="N17" s="2"/>
     </row>
   </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="C4:C13" sheet="December" r:id="rId1"/>
+    </dataRefs>
+  </dataConsolidate>
   <mergeCells count="2">
     <mergeCell ref="B2:K4"/>
     <mergeCell ref="L2:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1244,117 +1557,117 @@
   <dimension ref="B3:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+    <row r="3" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>40</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>32</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>31</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>36</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>35</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>30</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>33</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>38</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>37</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="18" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>34</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>39</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>38</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+    <row r="8" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>38</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
         <v>32</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>40</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>34</v>
       </c>
     </row>
@@ -1368,116 +1681,116 @@
   <dimension ref="B3:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="4" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="4" width="17.36328125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+    <row r="3" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>37</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>46</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>43</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>35</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>48</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>46</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>38</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>47</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>48</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="18" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>36</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>43</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>49</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+    <row r="8" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>31</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
         <v>41</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>50</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>46</v>
       </c>
     </row>
@@ -1490,144 +1803,146 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A978F9-C0A9-4E1D-BCBC-2E778433ED62}">
   <dimension ref="C2:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="31.33203125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="25.5546875" customWidth="1"/>
-    <col min="12" max="12" width="6.33203125" customWidth="1"/>
-    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="31.36328125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" customWidth="1"/>
+    <col min="12" max="12" width="6.36328125" customWidth="1"/>
+    <col min="13" max="13" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C2" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="2" t="s">
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="3:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="22" t="s">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="22"/>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="22"/>
+    </row>
+    <row r="5" spans="3:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="23"/>
-    </row>
-    <row r="6" spans="3:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="22" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="25"/>
+    </row>
+    <row r="6" spans="3:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="23"/>
-    </row>
-    <row r="7" spans="3:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="24" t="s">
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="25"/>
+    </row>
+    <row r="7" spans="3:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="26"/>
-    </row>
-    <row r="8" spans="3:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-    </row>
-    <row r="9" spans="3:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C9" s="30" t="s">
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="28"/>
+    </row>
+    <row r="8" spans="3:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" spans="3:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="C9" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="31"/>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-    </row>
-    <row r="11" spans="3:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C11" s="30" t="s">
+      <c r="D9" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+    </row>
+    <row r="11" spans="3:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="C11" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="31"/>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-    </row>
-    <row r="13" spans="3:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C13" s="30" t="s">
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="3:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="C13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="31"/>
+      <c r="D13" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1637,6 +1952,18 @@
     <mergeCell ref="C6:M6"/>
     <mergeCell ref="C7:M7"/>
   </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9" xr:uid="{AA57DAA4-B758-4BB9-968B-DC351FA30D4D}">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13" xr:uid="{DC89269D-056A-46E8-940F-B19B283B0DC4}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11" xr:uid="{27D8F652-F837-451E-A974-DF85D393B70A}">
+      <formula1>"C++, Python, R, Java, HTML"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1650,97 +1977,97 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="2:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="2:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="7">
         <v>82875</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="2:3" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="8">
         <v>42500</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="2:3" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="8">
         <v>24150</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="2:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="8">
         <v>22575</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="8">
         <v>23625</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="8">
         <v>19250</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="8">
         <v>9000</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="8">
         <v>3185.0000000000005</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="8">
         <v>23625</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="8">
         <v>7000</v>
       </c>
     </row>
@@ -1753,101 +2080,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5B7B35-DE42-466C-8CAA-1693800A6735}">
   <dimension ref="B3:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="2:3" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="2:3" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="9">
         <v>15937.5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="2:3" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="10">
         <v>19910</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="2:3" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="10">
         <v>7425</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="10">
         <v>10353</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:3" ht="25.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="10">
         <v>6875</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="2:3" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="10">
         <v>15750</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="2:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="10">
         <v>8002.5</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="2:3" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="10">
         <v>15562.5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="2:3" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="10">
         <v>65875</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="10">
         <v>38250</v>
       </c>
     </row>
@@ -1864,97 +2191,97 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="9">
         <v>10800</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="10">
         <v>53125</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="10">
         <v>23750</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="10">
         <v>7062.5</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="10">
         <v>17040</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="10">
         <v>7837.5</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="10">
         <v>63750</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="10">
         <v>6781.25</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="10">
         <v>16276.75</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="10">
         <v>2940</v>
       </c>
     </row>
@@ -1971,97 +2298,97 @@
       <selection activeCell="B3" sqref="B3:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="9">
         <v>16625</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="10">
         <v>14910</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="10">
         <v>18150</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="10">
         <v>7425</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="10">
         <v>6562.5</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="10">
         <v>6075</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="10">
         <v>15087.5</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="10">
         <v>63000</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="10">
         <v>6125</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="10">
         <v>3705</v>
       </c>
     </row>
@@ -2078,97 +2405,97 @@
       <selection activeCell="B3" sqref="B3:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="9">
         <v>6937.5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="10">
         <v>6277.5</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="10">
         <v>14910</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="10">
         <v>58800</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="10">
         <v>61625</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="10">
         <v>6750</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="10">
         <v>42000</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="10">
         <v>4562.5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="10">
         <v>7062.5</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="10">
         <v>76500</v>
       </c>
     </row>
@@ -2185,97 +2512,97 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="13.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C3" s="10" t="s">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C4" s="10" t="s">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="9">
         <v>3847.5</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C5" s="10" t="s">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="10">
         <v>4425</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C6" s="10" t="s">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="10">
         <v>17250</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C7" s="10" t="s">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="10">
         <v>5292.5</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C8" s="10" t="s">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="10">
         <v>7245.25</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C9" s="10" t="s">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="10">
         <v>13650</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C10" s="10" t="s">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="10">
         <v>3562.5</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C11" s="10" t="s">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="10">
         <v>3300</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C12" s="10" t="s">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="10">
         <v>16330</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C13" s="10" t="s">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="10">
         <v>5365.5</v>
       </c>
     </row>
@@ -2286,63 +2613,200 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37FD2D00-4B5E-41C0-8E1B-350E752EE76C}">
-  <dimension ref="B2:L4"/>
+  <dimension ref="A2:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="6" width="8.88671875" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="4" max="4" width="27.7265625" customWidth="1"/>
+    <col min="5" max="5" width="27.90625" customWidth="1"/>
+    <col min="6" max="6" width="28.36328125" customWidth="1"/>
+    <col min="12" max="12" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:12" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="2" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="2"/>
+    <row r="3" spans="1:12" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="39"/>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>108</v>
+      </c>
+      <c r="E7">
+        <v>106</v>
+      </c>
+      <c r="F7">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="39"/>
+      <c r="C8">
+        <v>83</v>
+      </c>
+      <c r="D8">
+        <v>110</v>
+      </c>
+      <c r="E8">
+        <v>98</v>
+      </c>
+      <c r="F8">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B9" s="39"/>
+      <c r="C9">
+        <v>87</v>
+      </c>
+      <c r="D9">
+        <v>113</v>
+      </c>
+      <c r="E9">
+        <v>109</v>
+      </c>
+      <c r="F9">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B10" s="39"/>
+      <c r="C10">
+        <v>87</v>
+      </c>
+      <c r="D10">
+        <v>103</v>
+      </c>
+      <c r="E10">
+        <v>112</v>
+      </c>
+      <c r="F10">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B11" s="39"/>
+      <c r="C11">
+        <v>94</v>
+      </c>
+      <c r="D11">
+        <v>105</v>
+      </c>
+      <c r="E11">
+        <v>118</v>
+      </c>
+      <c r="F11">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B12" s="39"/>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>24</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13">
+        <f>SUM(C7:C12)</f>
+        <v>471</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:F13" si="0">SUM(D7:D12)</f>
+        <v>563</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>563</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>613</v>
+      </c>
     </row>
   </sheetData>
-  <dataConsolidate leftLabels="1" topLabels="1"/>
+  <dataConsolidate topLabels="1">
+    <dataRefs count="3">
+      <dataRef ref="B3:F9" sheet="AZ Report"/>
+      <dataRef ref="B3:F8" sheet="IL Report"/>
+      <dataRef ref="B3:F8" sheet="NY Report"/>
+    </dataRefs>
+  </dataConsolidate>
   <mergeCells count="2">
     <mergeCell ref="B2:K4"/>
     <mergeCell ref="L2:L4"/>
@@ -2356,134 +2820,134 @@
   <dimension ref="B3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="4" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="3" max="4" width="13.453125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+    <row r="3" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B4" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>23</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>30</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>32</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>12</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>27</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>22</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>16</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>28</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>24</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="18" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B7" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>17</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>21</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>25</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>25</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
         <v>32</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>28</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="18" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B9" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>20</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="1">
         <v>24</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>20</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="1">
         <v>25</v>
       </c>
     </row>

</xml_diff>